<commit_message>
### 0.9.1 - [Bug] Solve cannot convert Cell value to Nullable<T> (issue #138)
</commit_message>
<xml_diff>
--- a/samples/xlsx/TestIssue138.xlsx
+++ b/samples/xlsx/TestIssue138.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\MiniExcel\samples\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F6C09C8-F7BF-499B-8419-9E22E96BF6A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B2750D2-7D79-473E-8104-D515C4E8BCF9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{820902AF-269B-48ED-AA7B-732A911EF1DC}"/>
+    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13290" xr2:uid="{820902AF-269B-48ED-AA7B-732A911EF1DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>date</t>
   </si>
@@ -58,12 +58,6 @@
   </si>
   <si>
     <t>測試商品1</t>
-  </si>
-  <si>
-    <t>測試商品2</t>
-  </si>
-  <si>
-    <t>測試商品3</t>
   </si>
 </sst>
 </file>
@@ -419,7 +413,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -479,7 +473,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>44257</v>
+        <v>44256</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -488,7 +482,7 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4">
         <v>111.11</v>
@@ -502,7 +496,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>44258</v>
+        <v>44256</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -511,7 +505,7 @@
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E7">
         <v>111.11</v>

</xml_diff>

<commit_message>
Code Refacturing & document fix
</commit_message>
<xml_diff>
--- a/samples/xlsx/TestIssue138.xlsx
+++ b/samples/xlsx/TestIssue138.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\MiniExcel\samples\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B2750D2-7D79-473E-8104-D515C4E8BCF9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A808E395-4982-4879-9EBB-C5064E256338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13290" xr2:uid="{820902AF-269B-48ED-AA7B-732A911EF1DC}"/>
+    <workbookView xWindow="-12990" yWindow="5550" windowWidth="7200" windowHeight="4830" xr2:uid="{820902AF-269B-48ED-AA7B-732A911EF1DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
-    <t>date</t>
-  </si>
-  <si>
     <t>實單每日損益</t>
   </si>
   <si>
@@ -58,6 +55,9 @@
   </si>
   <si>
     <t>測試商品1</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -413,7 +413,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -427,25 +427,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -459,7 +459,7 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2">
         <v>111.11</v>
@@ -482,7 +482,7 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E4">
         <v>111.11</v>
@@ -505,7 +505,7 @@
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E7">
         <v>111.11</v>

</xml_diff>